<commit_message>
All The Requirements are Done!Results are also Looking Awsome
</commit_message>
<xml_diff>
--- a/HList.xlsx
+++ b/HList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DataStructure AlgoINFO6205\assignments\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC6390F-09FE-4465-B441-A3E97D36EC49}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343A71F9-69B2-4FC5-B993-89F505366145}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="Group">Sheet1!$E:$E</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="95">
   <si>
     <t>Activities</t>
   </si>
@@ -224,13 +224,97 @@
   </si>
   <si>
     <t>Array</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eating Ice Cream </t>
+  </si>
+  <si>
+    <t>Getting News Update</t>
+  </si>
+  <si>
+    <t>Reading Magazine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing Mobile Games </t>
+  </si>
+  <si>
+    <t>Doing TODO  Activities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visting Doctor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing board Games </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ArtWork </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visiting Friend </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Going out for a coffee </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planning daily Activities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculating Budget </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Management </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visiting Pub </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attending Concert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experience Live Show </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Going out of Walk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swimming </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visiting Museum </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ice-Skating </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camping </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Sitting </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Farming </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baking Cookies </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safety procedures </t>
+  </si>
+  <si>
+    <t>Religious observerence</t>
+  </si>
+  <si>
+    <t>health management</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,8 +322,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,6 +339,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,9 +361,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,9 +704,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -641,743 +741,1135 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="C5">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
       <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C8">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="C9">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>32</v>
+        <v>1.65</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="C12">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C13">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C14">
         <v>30</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>5</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="D16">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>2.35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="D20">
+        <v>2.5499999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>68</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21">
+        <v>15</v>
+      </c>
+      <c r="D21">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22">
+        <v>30</v>
+      </c>
+      <c r="D22">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>71</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>30</v>
+      </c>
+      <c r="D24">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="D17">
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26">
+        <v>45</v>
+      </c>
+      <c r="D26">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27">
+        <v>30</v>
+      </c>
+      <c r="D27">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>74</v>
+      </c>
+      <c r="B28" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18">
-        <v>30</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D28">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29">
         <v>5</v>
       </c>
-      <c r="F18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19">
-        <v>30</v>
-      </c>
-      <c r="D19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20">
+      <c r="D29">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="C30">
         <v>5</v>
       </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21">
-        <v>60</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22">
-        <v>60</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23">
-        <v>60</v>
-      </c>
-      <c r="D23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24">
-        <v>15</v>
-      </c>
-      <c r="D24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25">
-        <v>45</v>
-      </c>
-      <c r="D25">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26">
-        <v>15</v>
-      </c>
-      <c r="D26">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27">
-        <v>45</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="F27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28">
-        <v>15</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="C29">
-        <v>45</v>
-      </c>
-      <c r="D29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30">
-        <v>45</v>
-      </c>
       <c r="D30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="C31">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3.65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C33">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="D33">
-        <v>7</v>
+        <v>4.2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34">
-        <v>45</v>
+        <v>54</v>
+      </c>
+      <c r="C34" s="2">
+        <v>5</v>
       </c>
       <c r="D34">
-        <v>7</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C35">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36">
         <v>45</v>
       </c>
-      <c r="C36">
-        <v>60</v>
-      </c>
       <c r="D36">
-        <v>7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C37">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D37">
-        <v>7</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>15</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C39">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="D39">
-        <v>7</v>
+        <v>5.4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="C40">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="D40">
-        <v>7.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C41">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D41">
-        <v>7.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="C42">
-        <v>120</v>
+        <v>30</v>
       </c>
       <c r="D42">
-        <v>7.5</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43" t="s">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
       <c r="C43">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D43">
-        <v>8</v>
-      </c>
-      <c r="F43" t="s">
-        <v>49</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="C44">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D44">
-        <v>8</v>
-      </c>
-      <c r="E44" t="s">
-        <v>13</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C45">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D45">
-        <v>8</v>
-      </c>
-      <c r="E45" t="s">
-        <v>18</v>
+        <v>5.95</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C46">
         <v>30</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47">
-        <v>60</v>
+        <v>12</v>
+      </c>
+      <c r="C47" s="3">
+        <v>30</v>
       </c>
       <c r="D47">
-        <v>8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
+        <v>18</v>
+      </c>
+      <c r="B48" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" s="3">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>19</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" s="3">
+        <v>60</v>
+      </c>
+      <c r="D49">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="3">
+        <v>60</v>
+      </c>
+      <c r="D50">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>21</v>
+      </c>
+      <c r="B51" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="3">
+        <v>60</v>
+      </c>
+      <c r="D51">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="3">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>23</v>
+      </c>
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="3">
+        <v>45</v>
+      </c>
+      <c r="D53">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>24</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>34</v>
+      </c>
+      <c r="B55" t="s">
+        <v>45</v>
+      </c>
+      <c r="C55" s="3">
+        <v>60</v>
+      </c>
+      <c r="D55">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>35</v>
+      </c>
+      <c r="B56" t="s">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C56" s="3">
+        <v>60</v>
+      </c>
+      <c r="D56">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>25</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="3">
+        <v>45</v>
+      </c>
+      <c r="D57">
+        <v>7.2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>40</v>
+      </c>
+      <c r="B58" t="s">
+        <v>17</v>
+      </c>
+      <c r="C58">
+        <v>120</v>
+      </c>
+      <c r="D58">
+        <v>7.24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>26</v>
       </c>
-      <c r="C48">
-        <v>15</v>
-      </c>
-      <c r="D48">
+      <c r="B59" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59">
+        <v>15</v>
+      </c>
+      <c r="D59">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="D60">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61">
+        <v>15</v>
+      </c>
+      <c r="D61">
+        <v>7.45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62">
+        <v>45</v>
+      </c>
+      <c r="D62">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>39</v>
+      </c>
+      <c r="B63" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63">
+        <v>45</v>
+      </c>
+      <c r="D63">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64">
+        <v>15</v>
+      </c>
+      <c r="D64">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>36</v>
+      </c>
+      <c r="B65" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65">
+        <v>15</v>
+      </c>
+      <c r="D65">
+        <v>7.65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="C66">
+        <v>45</v>
+      </c>
+      <c r="D66">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>30</v>
+      </c>
+      <c r="B67" t="s">
+        <v>37</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>37</v>
+      </c>
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68">
+        <v>120</v>
+      </c>
+      <c r="D68">
+        <v>7.85</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>31</v>
+      </c>
+      <c r="B69" t="s">
+        <v>23</v>
+      </c>
+      <c r="C69">
+        <v>15</v>
+      </c>
+      <c r="D69">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>32</v>
+      </c>
+      <c r="B70" t="s">
+        <v>28</v>
+      </c>
+      <c r="C70">
+        <v>45</v>
+      </c>
+      <c r="D70">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>41</v>
+      </c>
+      <c r="B71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71">
+        <v>45</v>
+      </c>
+      <c r="D71">
         <v>8</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F71" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>46</v>
+      </c>
+      <c r="B72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C72">
+        <v>15</v>
+      </c>
+      <c r="D72">
+        <v>8.1</v>
+      </c>
+      <c r="E72" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E73" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B74" t="s">
         <v>27</v>
       </c>
-      <c r="C49">
+      <c r="C74">
         <v>45</v>
       </c>
-      <c r="D49">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="D74">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>43</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75">
+        <v>30</v>
+      </c>
+      <c r="D75">
+        <v>8.4</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>44</v>
+      </c>
+      <c r="B76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76">
+        <v>30</v>
+      </c>
+      <c r="D76">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>45</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77">
+        <v>60</v>
+      </c>
+      <c r="D77">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B78" t="s">
         <v>10</v>
       </c>
-      <c r="C50">
-        <v>15</v>
-      </c>
-      <c r="D50">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="C78">
+        <v>15</v>
+      </c>
+      <c r="D78">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>49</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C51">
+      <c r="C79">
         <v>960</v>
       </c>
-      <c r="D51">
+      <c r="D79">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F51">
-    <sortCondition ref="A1"/>
+  <sortState ref="A2:F79">
+    <sortCondition ref="D1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>